<commit_message>
update nguồn khách hàng vs vị tri bán chạy
</commit_message>
<xml_diff>
--- a/WEB.CMS/wwwroot/Template/import/template-khach-hang-source.xlsx
+++ b/WEB.CMS/wwwroot/Template/import/template-khach-hang-source.xlsx
@@ -25,9 +25,6 @@
     <t xml:space="preserve">Số điện thoại </t>
   </si>
   <si>
-    <t>Ghi chú</t>
-  </si>
-  <si>
     <t>hieu</t>
   </si>
   <si>
@@ -35,6 +32,9 @@
   </si>
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>Nhu cầu</t>
   </si>
 </sst>
 </file>
@@ -390,7 +390,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -409,21 +409,21 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="C2">
         <v>123456789</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>